<commit_message>
test config file : remove 1 home from group 2
</commit_message>
<xml_diff>
--- a/sensors/FluksoConfigurations/FluksoTechnical_config1.xlsx
+++ b/sensors/FluksoConfigurations/FluksoTechnical_config1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halex\Documents\ULB\VDE\Voisin-d-energie-ULB\sensors\Flukso Configurations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halex\Documents\ULB\VDE\Voisin-d-energie-ULB\sensors\FluksoConfigurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782A6314-8780-4A2B-881F-6069F3234371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D51AFE-2AB8-4877-A9C1-6F12595DBE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="165" windowWidth="15585" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="408">
   <si>
     <t>Date</t>
   </si>
@@ -3267,10 +3267,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3430,14 +3430,6 @@
       </c>
       <c r="B19" s="1" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>2</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3852,7 +3844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>

</xml_diff>